<commit_message>
Chỉnh lại danh sách linh kiện
</commit_message>
<xml_diff>
--- a/Docs/OnePhaseController.xlsx
+++ b/Docs/OnePhaseController.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="108">
   <si>
     <t>LED1</t>
   </si>
@@ -335,13 +335,16 @@
   </si>
   <si>
     <t>Cổng AND dán</t>
+  </si>
+  <si>
+    <t>10K 5% WXD3-13-2W</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,6 +356,12 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -405,7 +414,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -707,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,7 +975,7 @@
         <v>80</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>27</v>
@@ -975,7 +984,7 @@
         <v>91</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
@@ -1294,8 +1303,15 @@
       <c r="D29" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+      <c r="E29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>